<commit_message>
all algos + new result form
</commit_message>
<xml_diff>
--- a/Multicriteria/bin/Debug/_test.xlsx
+++ b/Multicriteria/bin/Debug/_test.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Сравнительные характеристики" sheetId="1" r:id="Rd5029177781341f4"/>
-    <sheet name="System" sheetId="2" r:id="R5ec2796f7c9d44d7"/>
+    <sheet name="Сравнительные характеристики" sheetId="1" r:id="R6d36f34603144125"/>
+    <sheet name="System" sheetId="2" r:id="Reead983f5d9142c4"/>
   </sheets>
   <d:definedNames xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </workbook>
@@ -208,10 +208,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="0">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C3" s="0">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">

</xml_diff>